<commit_message>
Issue #390 WIP: Add pending specs
</commit_message>
<xml_diff>
--- a/spec/support/data/minimal_metadata/470 PDSC_minimal_metadataxls.xlsx
+++ b/spec/support/data/minimal_metadata/470 PDSC_minimal_metadataxls.xlsx
@@ -260,10 +260,10 @@
     <t xml:space="preserve">Nius blong Santo ribelion we Jimi Stevens i tekem ova Santo taon long May 28th 1980, </t>
   </si>
   <si>
-    <t>English|German</t>
-  </si>
-  <si>
-    <t>Mandarin|Cantonese</t>
+    <t>eng|German</t>
+  </si>
+  <si>
+    <t>cmn|Cantonese</t>
   </si>
   <si>
     <t>AD|AF</t>

</xml_diff>